<commit_message>
Fix grade export cutoffs
</commit_message>
<xml_diff>
--- a/samples/GradeCurve_Report_bob-grades.xlsx.xlsx
+++ b/samples/GradeCurve_Report_bob-grades.xlsx.xlsx
@@ -400,55 +400,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H96"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="str">
+        <v>Student Anonymous ID#</v>
+      </c>
+      <c r="B1" s="1" t="str">
         <v>MC</v>
       </c>
-      <c r="B1" s="1" t="str">
+      <c r="C1" s="1" t="str">
         <v>Essay</v>
       </c>
-      <c r="C1" s="1" t="str">
+      <c r="D1" s="1" t="str">
         <v>Total</v>
       </c>
-      <c r="D1" s="1" t="str">
+      <c r="E1" s="1" t="str">
         <v>Grade Mode</v>
       </c>
-      <c r="E1" s="1" t="str">
+      <c r="F1" s="1" t="str">
         <v>Degree</v>
       </c>
-      <c r="F1" s="1" t="str">
+      <c r="G1" s="1" t="str">
         <v>Scenario 1 Grade</v>
       </c>
-      <c r="G1" s="1" t="str">
+      <c r="H1" s="1" t="str">
         <v>Scenario 2 Grade</v>
       </c>
-      <c r="H1" s="1" t="str">
+      <c r="I1" s="1" t="str">
         <v>Scenario 3 Grade</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
+      <c r="A2" s="1" t="str">
+        <v>56015</v>
+      </c>
+      <c r="B2" s="1">
         <v>40</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>57</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>97</v>
       </c>
-      <c r="D2" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E2" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F2" s="1" t="str">
-        <v>A+</v>
+        <v>JD</v>
       </c>
       <c r="G2" s="1" t="str">
         <v>A+</v>
@@ -456,25 +459,28 @@
       <c r="H2" s="1" t="str">
         <v>A+</v>
       </c>
+      <c r="I2" s="1" t="str">
+        <v>A+</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="1">
+      <c r="A3" s="1" t="str">
+        <v>57830</v>
+      </c>
+      <c r="B3" s="1">
         <v>40</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <v>57</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>97</v>
       </c>
-      <c r="D3" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E3" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F3" s="1" t="str">
-        <v>A+</v>
+        <v>JD</v>
       </c>
       <c r="G3" s="1" t="str">
         <v>A+</v>
@@ -482,233 +488,260 @@
       <c r="H3" s="1" t="str">
         <v>A+</v>
       </c>
+      <c r="I3" s="1" t="str">
+        <v>A+</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="1">
-        <v>38</v>
+      <c r="A4" s="1" t="str">
+        <v>59056</v>
       </c>
       <c r="B4" s="1">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1">
         <v>53</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>91</v>
       </c>
-      <c r="D4" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E4" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F4" s="1" t="str">
-        <v>A</v>
+        <v>JD</v>
       </c>
       <c r="G4" s="1" t="str">
-        <v>A</v>
+        <v>A+</v>
       </c>
       <c r="H4" s="1" t="str">
         <v>A</v>
       </c>
+      <c r="I4" s="1" t="str">
+        <v>A</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="1">
-        <v>38</v>
+      <c r="A5" s="1" t="str">
+        <v>50520</v>
       </c>
       <c r="B5" s="1">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1">
         <v>52</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>90</v>
       </c>
-      <c r="D5" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E5" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F5" s="1" t="str">
+        <v>JD</v>
+      </c>
+      <c r="G5" s="1" t="str">
         <v>A</v>
       </c>
-      <c r="G5" s="1" t="str">
-        <v>A-</v>
-      </c>
       <c r="H5" s="1" t="str">
-        <v>A-</v>
+        <v>A</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <v>A</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1">
-        <v>38</v>
+      <c r="A6" s="1" t="str">
+        <v>59033</v>
       </c>
       <c r="B6" s="1">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1">
         <v>52</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>90</v>
       </c>
-      <c r="D6" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E6" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F6" s="1" t="str">
+        <v>JD</v>
+      </c>
+      <c r="G6" s="1" t="str">
         <v>A</v>
       </c>
-      <c r="G6" s="1" t="str">
-        <v>A-</v>
-      </c>
       <c r="H6" s="1" t="str">
-        <v>A-</v>
+        <v>A</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <v>A</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1">
+      <c r="A7" s="1" t="str">
+        <v>51101</v>
+      </c>
+      <c r="B7" s="1">
         <v>36</v>
       </c>
-      <c r="B7" s="1">
+      <c r="C7" s="1">
         <v>53</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>89</v>
       </c>
-      <c r="D7" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E7" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F7" s="1" t="str">
-        <v>A-</v>
+        <v>JD</v>
       </c>
       <c r="G7" s="1" t="str">
-        <v>A-</v>
+        <v>A</v>
       </c>
       <c r="H7" s="1" t="str">
-        <v>A-</v>
+        <v>A</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <v>A</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1">
-        <v>38</v>
+      <c r="A8" s="1" t="str">
+        <v>59417</v>
       </c>
       <c r="B8" s="1">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1">
         <v>51</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>89</v>
       </c>
-      <c r="D8" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E8" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F8" s="1" t="str">
-        <v>A-</v>
+        <v>JD</v>
       </c>
       <c r="G8" s="1" t="str">
-        <v>A-</v>
+        <v>A</v>
       </c>
       <c r="H8" s="1" t="str">
-        <v>A-</v>
+        <v>A</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <v>A</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1">
+      <c r="A9" s="1" t="str">
+        <v>59784</v>
+      </c>
+      <c r="B9" s="1">
         <v>36</v>
       </c>
-      <c r="B9" s="1">
+      <c r="C9" s="1">
         <v>52</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>88</v>
       </c>
-      <c r="D9" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E9" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F9" s="1" t="str">
-        <v>A-</v>
+        <v>JD</v>
       </c>
       <c r="G9" s="1" t="str">
-        <v>A-</v>
+        <v>A</v>
       </c>
       <c r="H9" s="1" t="str">
-        <v>A-</v>
+        <v>A</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <v>A</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1">
+      <c r="A10" s="1" t="str">
+        <v>53793</v>
+      </c>
+      <c r="B10" s="1">
         <v>32</v>
       </c>
-      <c r="B10" s="1">
+      <c r="C10" s="1">
         <v>55</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>87</v>
       </c>
-      <c r="D10" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E10" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F10" s="1" t="str">
-        <v>A-</v>
+        <v>JD</v>
       </c>
       <c r="G10" s="1" t="str">
-        <v>A-</v>
+        <v>A</v>
       </c>
       <c r="H10" s="1" t="str">
-        <v>A-</v>
+        <v>A</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <v>A</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1">
-        <v>38</v>
+      <c r="A11" s="1" t="str">
+        <v>57795</v>
       </c>
       <c r="B11" s="1">
+        <v>38</v>
+      </c>
+      <c r="C11" s="1">
         <v>49</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>87</v>
       </c>
-      <c r="D11" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E11" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F11" s="1" t="str">
-        <v>A-</v>
+        <v>JD</v>
       </c>
       <c r="G11" s="1" t="str">
-        <v>A-</v>
+        <v>A</v>
       </c>
       <c r="H11" s="1" t="str">
-        <v>A-</v>
+        <v>A</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <v>A</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1">
-        <v>38</v>
+      <c r="A12" s="1" t="str">
+        <v>51883</v>
       </c>
       <c r="B12" s="1">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1">
         <v>48</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>86</v>
       </c>
-      <c r="D12" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E12" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F12" s="1" t="str">
-        <v>A-</v>
+        <v>JD</v>
       </c>
       <c r="G12" s="1" t="str">
         <v>A-</v>
@@ -716,25 +749,28 @@
       <c r="H12" s="1" t="str">
         <v>A-</v>
       </c>
+      <c r="I12" s="1" t="str">
+        <v>A-</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="1">
+      <c r="A13" s="1" t="str">
+        <v>56371</v>
+      </c>
+      <c r="B13" s="1">
         <v>40</v>
       </c>
-      <c r="B13" s="1">
+      <c r="C13" s="1">
         <v>46</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>86</v>
       </c>
-      <c r="D13" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E13" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F13" s="1" t="str">
-        <v>A-</v>
+        <v>JD</v>
       </c>
       <c r="G13" s="1" t="str">
         <v>A-</v>
@@ -742,25 +778,28 @@
       <c r="H13" s="1" t="str">
         <v>A-</v>
       </c>
+      <c r="I13" s="1" t="str">
+        <v>A-</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="1">
-        <v>38</v>
+      <c r="A14" s="1" t="str">
+        <v>57712</v>
       </c>
       <c r="B14" s="1">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1">
         <v>48</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>86</v>
       </c>
-      <c r="D14" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E14" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F14" s="1" t="str">
-        <v>A-</v>
+        <v>JD</v>
       </c>
       <c r="G14" s="1" t="str">
         <v>A-</v>
@@ -768,25 +807,28 @@
       <c r="H14" s="1" t="str">
         <v>A-</v>
       </c>
+      <c r="I14" s="1" t="str">
+        <v>A-</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="1">
-        <v>38</v>
+      <c r="A15" s="1" t="str">
+        <v>59513</v>
       </c>
       <c r="B15" s="1">
+        <v>38</v>
+      </c>
+      <c r="C15" s="1">
         <v>48</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>86</v>
       </c>
-      <c r="D15" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E15" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F15" s="1" t="str">
-        <v>A-</v>
+        <v>JD</v>
       </c>
       <c r="G15" s="1" t="str">
         <v>A-</v>
@@ -794,415 +836,463 @@
       <c r="H15" s="1" t="str">
         <v>A-</v>
       </c>
+      <c r="I15" s="1" t="str">
+        <v>A-</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="1">
+      <c r="A16" s="1" t="str">
+        <v>52102</v>
+      </c>
+      <c r="B16" s="1">
         <v>40</v>
       </c>
-      <c r="B16" s="1">
+      <c r="C16" s="1">
         <v>45</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>85</v>
       </c>
-      <c r="D16" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E16" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F16" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G16" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H16" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1">
-        <v>38</v>
+      <c r="A17" s="1" t="str">
+        <v>52926</v>
       </c>
       <c r="B17" s="1">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1">
         <v>47</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>85</v>
       </c>
-      <c r="D17" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E17" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F17" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G17" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H17" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1">
-        <v>38</v>
+      <c r="A18" s="1" t="str">
+        <v>53691</v>
       </c>
       <c r="B18" s="1">
+        <v>38</v>
+      </c>
+      <c r="C18" s="1">
         <v>47</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>85</v>
       </c>
-      <c r="D18" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E18" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F18" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G18" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H18" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1">
+      <c r="A19" s="1" t="str">
+        <v>53841</v>
+      </c>
+      <c r="B19" s="1">
         <v>40</v>
       </c>
-      <c r="B19" s="1">
+      <c r="C19" s="1">
         <v>45</v>
       </c>
-      <c r="C19" s="1">
+      <c r="D19" s="1">
         <v>85</v>
       </c>
-      <c r="D19" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E19" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F19" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G19" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H19" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1">
+      <c r="A20" s="1" t="str">
+        <v>51778</v>
+      </c>
+      <c r="B20" s="1">
         <v>34</v>
       </c>
-      <c r="B20" s="1">
+      <c r="C20" s="1">
         <v>50</v>
       </c>
-      <c r="C20" s="1">
+      <c r="D20" s="1">
         <v>84</v>
       </c>
-      <c r="D20" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E20" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F20" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G20" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H20" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1">
+      <c r="A21" s="1" t="str">
+        <v>51973</v>
+      </c>
+      <c r="B21" s="1">
         <v>36</v>
       </c>
-      <c r="B21" s="1">
+      <c r="C21" s="1">
         <v>48</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <v>84</v>
       </c>
-      <c r="D21" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E21" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F21" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G21" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H21" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1">
+      <c r="A22" s="1" t="str">
+        <v>53310</v>
+      </c>
+      <c r="B22" s="1">
         <v>36</v>
       </c>
-      <c r="B22" s="1">
+      <c r="C22" s="1">
         <v>48</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D22" s="1">
         <v>84</v>
       </c>
-      <c r="D22" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E22" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F22" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G22" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H22" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1">
+      <c r="A23" s="1" t="str">
+        <v>54727</v>
+      </c>
+      <c r="B23" s="1">
         <v>36</v>
       </c>
-      <c r="B23" s="1">
+      <c r="C23" s="1">
         <v>48</v>
       </c>
-      <c r="C23" s="1">
+      <c r="D23" s="1">
         <v>84</v>
       </c>
-      <c r="D23" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E23" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F23" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G23" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H23" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1">
-        <v>38</v>
+      <c r="A24" s="1" t="str">
+        <v>57500</v>
       </c>
       <c r="B24" s="1">
+        <v>38</v>
+      </c>
+      <c r="C24" s="1">
         <v>46</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D24" s="1">
         <v>84</v>
       </c>
-      <c r="D24" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E24" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F24" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G24" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H24" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1">
+      <c r="A25" s="1" t="str">
+        <v>58803</v>
+      </c>
+      <c r="B25" s="1">
         <v>40</v>
       </c>
-      <c r="B25" s="1">
+      <c r="C25" s="1">
         <v>44</v>
       </c>
-      <c r="C25" s="1">
+      <c r="D25" s="1">
         <v>84</v>
       </c>
-      <c r="D25" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E25" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F25" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G25" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H25" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1">
+      <c r="A26" s="1" t="str">
+        <v>59137</v>
+      </c>
+      <c r="B26" s="1">
         <v>36</v>
       </c>
-      <c r="B26" s="1">
+      <c r="C26" s="1">
         <v>48</v>
       </c>
-      <c r="C26" s="1">
+      <c r="D26" s="1">
         <v>84</v>
       </c>
-      <c r="D26" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E26" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F26" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G26" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H26" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1">
+      <c r="A27" s="1" t="str">
+        <v>50591</v>
+      </c>
+      <c r="B27" s="1">
         <v>34</v>
       </c>
-      <c r="B27" s="1">
+      <c r="C27" s="1">
         <v>49</v>
       </c>
-      <c r="C27" s="1">
+      <c r="D27" s="1">
         <v>83</v>
       </c>
-      <c r="D27" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E27" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F27" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G27" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H27" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1">
+      <c r="A28" s="1" t="str">
+        <v>53517</v>
+      </c>
+      <c r="B28" s="1">
         <v>40</v>
       </c>
-      <c r="B28" s="1">
+      <c r="C28" s="1">
         <v>43</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D28" s="1">
         <v>83</v>
       </c>
-      <c r="D28" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E28" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F28" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G28" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H28" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1">
-        <v>38</v>
+      <c r="A29" s="1" t="str">
+        <v>55803</v>
       </c>
       <c r="B29" s="1">
+        <v>38</v>
+      </c>
+      <c r="C29" s="1">
         <v>45</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29" s="1">
         <v>83</v>
       </c>
-      <c r="D29" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E29" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F29" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G29" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H29" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1">
-        <v>38</v>
+      <c r="A30" s="1" t="str">
+        <v>59143</v>
       </c>
       <c r="B30" s="1">
+        <v>38</v>
+      </c>
+      <c r="C30" s="1">
         <v>45</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D30" s="1">
         <v>83</v>
       </c>
-      <c r="D30" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E30" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F30" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G30" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
       </c>
       <c r="H30" s="1" t="str">
-        <v>B+</v>
+        <v>A-</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <v>A-</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1">
+      <c r="A31" s="1" t="str">
+        <v>51474</v>
+      </c>
+      <c r="B31" s="1">
         <v>34</v>
       </c>
-      <c r="B31" s="1">
+      <c r="C31" s="1">
         <v>48</v>
       </c>
-      <c r="C31" s="1">
+      <c r="D31" s="1">
         <v>82</v>
       </c>
-      <c r="D31" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E31" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F31" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G31" s="1" t="str">
         <v>B+</v>
@@ -1210,25 +1300,28 @@
       <c r="H31" s="1" t="str">
         <v>B+</v>
       </c>
+      <c r="I31" s="1" t="str">
+        <v>B+</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="1">
+      <c r="A32" s="1" t="str">
+        <v>54189</v>
+      </c>
+      <c r="B32" s="1">
         <v>40</v>
       </c>
-      <c r="B32" s="1">
+      <c r="C32" s="1">
         <v>42</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="1">
         <v>82</v>
       </c>
-      <c r="D32" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E32" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F32" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G32" s="1" t="str">
         <v>B+</v>
@@ -1236,25 +1329,28 @@
       <c r="H32" s="1" t="str">
         <v>B+</v>
       </c>
+      <c r="I32" s="1" t="str">
+        <v>B+</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="1">
+      <c r="A33" s="1" t="str">
+        <v>54482</v>
+      </c>
+      <c r="B33" s="1">
         <v>36</v>
       </c>
-      <c r="B33" s="1">
+      <c r="C33" s="1">
         <v>46</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D33" s="1">
         <v>82</v>
       </c>
-      <c r="D33" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E33" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F33" s="1" t="str">
-        <v>B+</v>
+        <v>JD</v>
       </c>
       <c r="G33" s="1" t="str">
         <v>B+</v>
@@ -1262,753 +1358,840 @@
       <c r="H33" s="1" t="str">
         <v>B+</v>
       </c>
+      <c r="I33" s="1" t="str">
+        <v>B+</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="1">
-        <v>38</v>
+      <c r="A34" s="1" t="str">
+        <v>52111</v>
       </c>
       <c r="B34" s="1">
+        <v>38</v>
+      </c>
+      <c r="C34" s="1">
         <v>43</v>
       </c>
-      <c r="C34" s="1">
+      <c r="D34" s="1">
         <v>81</v>
       </c>
-      <c r="D34" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E34" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F34" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G34" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H34" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I34" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1">
+      <c r="A35" s="1" t="str">
+        <v>52842</v>
+      </c>
+      <c r="B35" s="1">
         <v>36</v>
       </c>
-      <c r="B35" s="1">
+      <c r="C35" s="1">
         <v>45</v>
       </c>
-      <c r="C35" s="1">
+      <c r="D35" s="1">
         <v>81</v>
       </c>
-      <c r="D35" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E35" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F35" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G35" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H35" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I35" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1">
-        <v>38</v>
+      <c r="A36" s="1" t="str">
+        <v>55248</v>
       </c>
       <c r="B36" s="1">
+        <v>38</v>
+      </c>
+      <c r="C36" s="1">
         <v>43</v>
       </c>
-      <c r="C36" s="1">
+      <c r="D36" s="1">
         <v>81</v>
       </c>
-      <c r="D36" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E36" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F36" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G36" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H36" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I36" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1">
-        <v>38</v>
+      <c r="A37" s="1" t="str">
+        <v>56733</v>
       </c>
       <c r="B37" s="1">
+        <v>38</v>
+      </c>
+      <c r="C37" s="1">
         <v>43</v>
       </c>
-      <c r="C37" s="1">
+      <c r="D37" s="1">
         <v>81</v>
       </c>
-      <c r="D37" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E37" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F37" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G37" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H37" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I37" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1">
+      <c r="A38" s="1" t="str">
+        <v>57170</v>
+      </c>
+      <c r="B38" s="1">
         <v>34</v>
       </c>
-      <c r="B38" s="1">
+      <c r="C38" s="1">
         <v>47</v>
       </c>
-      <c r="C38" s="1">
+      <c r="D38" s="1">
         <v>81</v>
       </c>
-      <c r="D38" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E38" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F38" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G38" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H38" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I38" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1">
+      <c r="A39" s="1" t="str">
+        <v>58770</v>
+      </c>
+      <c r="B39" s="1">
         <v>40</v>
       </c>
-      <c r="B39" s="1">
+      <c r="C39" s="1">
         <v>41</v>
       </c>
-      <c r="C39" s="1">
+      <c r="D39" s="1">
         <v>81</v>
       </c>
-      <c r="D39" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E39" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F39" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G39" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H39" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I39" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1">
+      <c r="A40" s="1" t="str">
+        <v>59908</v>
+      </c>
+      <c r="B40" s="1">
         <v>40</v>
       </c>
-      <c r="B40" s="1">
+      <c r="C40" s="1">
         <v>41</v>
       </c>
-      <c r="C40" s="1">
+      <c r="D40" s="1">
         <v>81</v>
       </c>
-      <c r="D40" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E40" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F40" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G40" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H40" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I40" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1">
-        <v>38</v>
+      <c r="A41" s="1" t="str">
+        <v>59939</v>
       </c>
       <c r="B41" s="1">
+        <v>38</v>
+      </c>
+      <c r="C41" s="1">
         <v>43</v>
       </c>
-      <c r="C41" s="1">
+      <c r="D41" s="1">
         <v>81</v>
       </c>
-      <c r="D41" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E41" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F41" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G41" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H41" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I41" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1">
-        <v>38</v>
+      <c r="A42" s="1" t="str">
+        <v>59943</v>
       </c>
       <c r="B42" s="1">
+        <v>38</v>
+      </c>
+      <c r="C42" s="1">
         <v>43</v>
       </c>
-      <c r="C42" s="1">
+      <c r="D42" s="1">
         <v>81</v>
       </c>
-      <c r="D42" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E42" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F42" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G42" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H42" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I42" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1">
-        <v>40</v>
+      <c r="A43" s="1" t="str">
+        <v>50118</v>
       </c>
       <c r="B43" s="1">
         <v>40</v>
       </c>
       <c r="C43" s="1">
+        <v>40</v>
+      </c>
+      <c r="D43" s="1">
         <v>80</v>
       </c>
-      <c r="D43" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E43" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F43" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G43" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H43" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I43" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1">
+      <c r="A44" s="1" t="str">
+        <v>50684</v>
+      </c>
+      <c r="B44" s="1">
         <v>36</v>
       </c>
-      <c r="B44" s="1">
+      <c r="C44" s="1">
         <v>44</v>
       </c>
-      <c r="C44" s="1">
+      <c r="D44" s="1">
         <v>80</v>
       </c>
-      <c r="D44" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E44" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F44" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G44" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H44" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I44" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1">
-        <v>38</v>
+      <c r="A45" s="1" t="str">
+        <v>52499</v>
       </c>
       <c r="B45" s="1">
+        <v>38</v>
+      </c>
+      <c r="C45" s="1">
         <v>42</v>
       </c>
-      <c r="C45" s="1">
+      <c r="D45" s="1">
         <v>80</v>
       </c>
-      <c r="D45" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E45" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F45" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G45" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H45" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I45" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1">
+      <c r="A46" s="1" t="str">
+        <v>53632</v>
+      </c>
+      <c r="B46" s="1">
         <v>36</v>
       </c>
-      <c r="B46" s="1">
+      <c r="C46" s="1">
         <v>44</v>
       </c>
-      <c r="C46" s="1">
+      <c r="D46" s="1">
         <v>80</v>
       </c>
-      <c r="D46" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E46" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F46" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G46" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H46" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I46" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1">
-        <v>38</v>
+      <c r="A47" s="1" t="str">
+        <v>58914</v>
       </c>
       <c r="B47" s="1">
+        <v>38</v>
+      </c>
+      <c r="C47" s="1">
         <v>42</v>
       </c>
-      <c r="C47" s="1">
+      <c r="D47" s="1">
         <v>80</v>
       </c>
-      <c r="D47" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E47" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F47" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G47" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H47" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I47" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1">
-        <v>38</v>
+      <c r="A48" s="1" t="str">
+        <v>51697</v>
       </c>
       <c r="B48" s="1">
+        <v>38</v>
+      </c>
+      <c r="C48" s="1">
         <v>41</v>
       </c>
-      <c r="C48" s="1">
+      <c r="D48" s="1">
         <v>79</v>
       </c>
-      <c r="D48" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E48" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F48" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G48" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H48" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I48" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1">
-        <v>38</v>
+      <c r="A49" s="1" t="str">
+        <v>55709</v>
       </c>
       <c r="B49" s="1">
+        <v>38</v>
+      </c>
+      <c r="C49" s="1">
         <v>41</v>
       </c>
-      <c r="C49" s="1">
+      <c r="D49" s="1">
         <v>79</v>
       </c>
-      <c r="D49" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E49" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F49" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G49" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H49" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I49" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1">
+      <c r="A50" s="1" t="str">
+        <v>58338</v>
+      </c>
+      <c r="B50" s="1">
         <v>36</v>
       </c>
-      <c r="B50" s="1">
+      <c r="C50" s="1">
         <v>43</v>
       </c>
-      <c r="C50" s="1">
+      <c r="D50" s="1">
         <v>79</v>
       </c>
-      <c r="D50" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E50" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F50" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G50" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H50" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I50" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1">
-        <v>38</v>
+      <c r="A51" s="1" t="str">
+        <v>52793</v>
       </c>
       <c r="B51" s="1">
+        <v>38</v>
+      </c>
+      <c r="C51" s="1">
         <v>40</v>
       </c>
-      <c r="C51" s="1">
+      <c r="D51" s="1">
         <v>78</v>
       </c>
-      <c r="D51" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E51" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F51" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G51" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H51" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I51" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1">
-        <v>38</v>
+      <c r="A52" s="1" t="str">
+        <v>53374</v>
       </c>
       <c r="B52" s="1">
+        <v>38</v>
+      </c>
+      <c r="C52" s="1">
         <v>40</v>
       </c>
-      <c r="C52" s="1">
+      <c r="D52" s="1">
         <v>78</v>
       </c>
-      <c r="D52" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E52" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F52" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G52" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H52" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I52" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1">
-        <v>38</v>
+      <c r="A53" s="1" t="str">
+        <v>54267</v>
       </c>
       <c r="B53" s="1">
+        <v>38</v>
+      </c>
+      <c r="C53" s="1">
         <v>40</v>
       </c>
-      <c r="C53" s="1">
+      <c r="D53" s="1">
         <v>78</v>
       </c>
-      <c r="D53" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E53" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F53" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G53" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H53" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I53" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1">
+      <c r="A54" s="1" t="str">
+        <v>54364</v>
+      </c>
+      <c r="B54" s="1">
         <v>40</v>
       </c>
-      <c r="B54" s="1">
-        <v>38</v>
-      </c>
       <c r="C54" s="1">
+        <v>38</v>
+      </c>
+      <c r="D54" s="1">
         <v>78</v>
       </c>
-      <c r="D54" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E54" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F54" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G54" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H54" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I54" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1">
+      <c r="A55" s="1" t="str">
+        <v>55863</v>
+      </c>
+      <c r="B55" s="1">
         <v>32</v>
       </c>
-      <c r="B55" s="1">
+      <c r="C55" s="1">
         <v>46</v>
       </c>
-      <c r="C55" s="1">
+      <c r="D55" s="1">
         <v>78</v>
       </c>
-      <c r="D55" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E55" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F55" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G55" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H55" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I55" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1">
-        <v>38</v>
+      <c r="A56" s="1" t="str">
+        <v>56175</v>
       </c>
       <c r="B56" s="1">
+        <v>38</v>
+      </c>
+      <c r="C56" s="1">
         <v>40</v>
       </c>
-      <c r="C56" s="1">
+      <c r="D56" s="1">
         <v>78</v>
       </c>
-      <c r="D56" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E56" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F56" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G56" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H56" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I56" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1">
+      <c r="A57" s="1" t="str">
+        <v>59707</v>
+      </c>
+      <c r="B57" s="1">
         <v>40</v>
       </c>
-      <c r="B57" s="1">
-        <v>38</v>
-      </c>
       <c r="C57" s="1">
+        <v>38</v>
+      </c>
+      <c r="D57" s="1">
         <v>78</v>
       </c>
-      <c r="D57" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E57" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F57" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G57" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H57" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I57" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1">
-        <v>38</v>
+      <c r="A58" s="1" t="str">
+        <v>50150</v>
       </c>
       <c r="B58" s="1">
+        <v>38</v>
+      </c>
+      <c r="C58" s="1">
         <v>39</v>
       </c>
-      <c r="C58" s="1">
+      <c r="D58" s="1">
         <v>77</v>
       </c>
-      <c r="D58" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E58" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F58" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G58" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H58" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I58" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1">
+      <c r="A59" s="1" t="str">
+        <v>52886</v>
+      </c>
+      <c r="B59" s="1">
         <v>34</v>
       </c>
-      <c r="B59" s="1">
+      <c r="C59" s="1">
         <v>43</v>
       </c>
-      <c r="C59" s="1">
+      <c r="D59" s="1">
         <v>77</v>
       </c>
-      <c r="D59" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E59" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F59" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G59" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H59" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I59" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1">
+      <c r="A60" s="1" t="str">
+        <v>57952</v>
+      </c>
+      <c r="B60" s="1">
         <v>36</v>
       </c>
-      <c r="B60" s="1">
+      <c r="C60" s="1">
         <v>41</v>
       </c>
-      <c r="C60" s="1">
+      <c r="D60" s="1">
         <v>77</v>
       </c>
-      <c r="D60" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E60" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F60" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G60" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H60" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I60" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1">
+      <c r="A61" s="1" t="str">
+        <v>58738</v>
+      </c>
+      <c r="B61" s="1">
         <v>36</v>
       </c>
-      <c r="B61" s="1">
+      <c r="C61" s="1">
         <v>41</v>
       </c>
-      <c r="C61" s="1">
+      <c r="D61" s="1">
         <v>77</v>
       </c>
-      <c r="D61" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E61" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F61" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G61" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H61" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I61" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1">
+      <c r="A62" s="1" t="str">
+        <v>52284</v>
+      </c>
+      <c r="B62" s="1">
         <v>32</v>
       </c>
-      <c r="B62" s="1">
+      <c r="C62" s="1">
         <v>44</v>
       </c>
-      <c r="C62" s="1">
+      <c r="D62" s="1">
         <v>76</v>
       </c>
-      <c r="D62" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E62" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F62" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G62" s="1" t="str">
         <v>B</v>
@@ -2016,25 +2199,28 @@
       <c r="H62" s="1" t="str">
         <v>B</v>
       </c>
+      <c r="I62" s="1" t="str">
+        <v>B</v>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" s="1">
-        <v>38</v>
+      <c r="A63" s="1" t="str">
+        <v>54958</v>
       </c>
       <c r="B63" s="1">
         <v>38</v>
       </c>
       <c r="C63" s="1">
+        <v>38</v>
+      </c>
+      <c r="D63" s="1">
         <v>76</v>
       </c>
-      <c r="D63" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E63" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F63" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G63" s="1" t="str">
         <v>B</v>
@@ -2042,25 +2228,28 @@
       <c r="H63" s="1" t="str">
         <v>B</v>
       </c>
+      <c r="I63" s="1" t="str">
+        <v>B</v>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" s="1">
-        <v>38</v>
+      <c r="A64" s="1" t="str">
+        <v>55146</v>
       </c>
       <c r="B64" s="1">
         <v>38</v>
       </c>
       <c r="C64" s="1">
+        <v>38</v>
+      </c>
+      <c r="D64" s="1">
         <v>76</v>
       </c>
-      <c r="D64" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E64" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F64" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G64" s="1" t="str">
         <v>B</v>
@@ -2068,25 +2257,28 @@
       <c r="H64" s="1" t="str">
         <v>B</v>
       </c>
+      <c r="I64" s="1" t="str">
+        <v>B</v>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" s="1">
-        <v>38</v>
+      <c r="A65" s="1" t="str">
+        <v>57243</v>
       </c>
       <c r="B65" s="1">
         <v>38</v>
       </c>
       <c r="C65" s="1">
+        <v>38</v>
+      </c>
+      <c r="D65" s="1">
         <v>76</v>
       </c>
-      <c r="D65" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E65" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F65" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G65" s="1" t="str">
         <v>B</v>
@@ -2094,25 +2286,28 @@
       <c r="H65" s="1" t="str">
         <v>B</v>
       </c>
+      <c r="I65" s="1" t="str">
+        <v>B</v>
+      </c>
     </row>
     <row r="66">
-      <c r="A66" s="1">
+      <c r="A66" s="1" t="str">
+        <v>58304</v>
+      </c>
+      <c r="B66" s="1">
         <v>36</v>
       </c>
-      <c r="B66" s="1">
+      <c r="C66" s="1">
         <v>40</v>
       </c>
-      <c r="C66" s="1">
+      <c r="D66" s="1">
         <v>76</v>
       </c>
-      <c r="D66" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E66" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F66" s="1" t="str">
-        <v>B</v>
+        <v>JD</v>
       </c>
       <c r="G66" s="1" t="str">
         <v>B</v>
@@ -2120,415 +2315,463 @@
       <c r="H66" s="1" t="str">
         <v>B</v>
       </c>
+      <c r="I66" s="1" t="str">
+        <v>B</v>
+      </c>
     </row>
     <row r="67">
-      <c r="A67" s="1">
+      <c r="A67" s="1" t="str">
+        <v>50239</v>
+      </c>
+      <c r="B67" s="1">
         <v>36</v>
       </c>
-      <c r="B67" s="1">
+      <c r="C67" s="1">
         <v>39</v>
       </c>
-      <c r="C67" s="1">
+      <c r="D67" s="1">
         <v>75</v>
       </c>
-      <c r="D67" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E67" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F67" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G67" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H67" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I67" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1">
+      <c r="A68" s="1" t="str">
+        <v>55080</v>
+      </c>
+      <c r="B68" s="1">
         <v>36</v>
       </c>
-      <c r="B68" s="1">
+      <c r="C68" s="1">
         <v>39</v>
       </c>
-      <c r="C68" s="1">
+      <c r="D68" s="1">
         <v>75</v>
       </c>
-      <c r="D68" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E68" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F68" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G68" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H68" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I68" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1">
+      <c r="A69" s="1" t="str">
+        <v>59554</v>
+      </c>
+      <c r="B69" s="1">
         <v>40</v>
       </c>
-      <c r="B69" s="1">
+      <c r="C69" s="1">
         <v>35</v>
       </c>
-      <c r="C69" s="1">
+      <c r="D69" s="1">
         <v>75</v>
       </c>
-      <c r="D69" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E69" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F69" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G69" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H69" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I69" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1">
+      <c r="A70" s="1" t="str">
+        <v>50964</v>
+      </c>
+      <c r="B70" s="1">
         <v>32</v>
       </c>
-      <c r="B70" s="1">
+      <c r="C70" s="1">
         <v>42</v>
       </c>
-      <c r="C70" s="1">
+      <c r="D70" s="1">
         <v>74</v>
       </c>
-      <c r="D70" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E70" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F70" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G70" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H70" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I70" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1">
-        <v>38</v>
+      <c r="A71" s="1" t="str">
+        <v>51014</v>
       </c>
       <c r="B71" s="1">
+        <v>38</v>
+      </c>
+      <c r="C71" s="1">
         <v>36</v>
       </c>
-      <c r="C71" s="1">
+      <c r="D71" s="1">
         <v>74</v>
       </c>
-      <c r="D71" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E71" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F71" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G71" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H71" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I71" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1">
+      <c r="A72" s="1" t="str">
+        <v>55186</v>
+      </c>
+      <c r="B72" s="1">
         <v>36</v>
       </c>
-      <c r="B72" s="1">
-        <v>38</v>
-      </c>
       <c r="C72" s="1">
+        <v>38</v>
+      </c>
+      <c r="D72" s="1">
         <v>74</v>
       </c>
-      <c r="D72" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E72" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F72" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G72" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H72" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I72" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1">
+      <c r="A73" s="1" t="str">
+        <v>55507</v>
+      </c>
+      <c r="B73" s="1">
         <v>34</v>
       </c>
-      <c r="B73" s="1">
+      <c r="C73" s="1">
         <v>40</v>
       </c>
-      <c r="C73" s="1">
+      <c r="D73" s="1">
         <v>74</v>
       </c>
-      <c r="D73" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E73" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F73" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G73" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H73" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I73" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1">
-        <v>38</v>
+      <c r="A74" s="1" t="str">
+        <v>50103</v>
       </c>
       <c r="B74" s="1">
+        <v>38</v>
+      </c>
+      <c r="C74" s="1">
         <v>35</v>
       </c>
-      <c r="C74" s="1">
+      <c r="D74" s="1">
         <v>73</v>
       </c>
-      <c r="D74" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E74" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F74" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G74" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H74" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I74" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1">
+      <c r="A75" s="1" t="str">
+        <v>50274</v>
+      </c>
+      <c r="B75" s="1">
         <v>34</v>
       </c>
-      <c r="B75" s="1">
+      <c r="C75" s="1">
         <v>39</v>
       </c>
-      <c r="C75" s="1">
+      <c r="D75" s="1">
         <v>73</v>
       </c>
-      <c r="D75" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E75" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F75" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G75" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H75" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I75" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1">
+      <c r="A76" s="1" t="str">
+        <v>56367</v>
+      </c>
+      <c r="B76" s="1">
         <v>36</v>
       </c>
-      <c r="B76" s="1">
+      <c r="C76" s="1">
         <v>37</v>
       </c>
-      <c r="C76" s="1">
+      <c r="D76" s="1">
         <v>73</v>
       </c>
-      <c r="D76" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E76" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F76" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G76" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H76" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I76" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1">
+      <c r="A77" s="1" t="str">
+        <v>53223</v>
+      </c>
+      <c r="B77" s="1">
         <v>30</v>
       </c>
-      <c r="B77" s="1">
+      <c r="C77" s="1">
         <v>42</v>
       </c>
-      <c r="C77" s="1">
+      <c r="D77" s="1">
         <v>72</v>
       </c>
-      <c r="D77" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E77" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F77" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G77" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H77" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I77" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1">
+      <c r="A78" s="1" t="str">
+        <v>56510</v>
+      </c>
+      <c r="B78" s="1">
         <v>34</v>
       </c>
-      <c r="B78" s="1">
-        <v>38</v>
-      </c>
       <c r="C78" s="1">
+        <v>38</v>
+      </c>
+      <c r="D78" s="1">
         <v>72</v>
       </c>
-      <c r="D78" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E78" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F78" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G78" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H78" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I78" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1">
+      <c r="A79" s="1" t="str">
+        <v>54649</v>
+      </c>
+      <c r="B79" s="1">
         <v>34</v>
       </c>
-      <c r="B79" s="1">
+      <c r="C79" s="1">
         <v>36</v>
       </c>
-      <c r="C79" s="1">
+      <c r="D79" s="1">
         <v>70</v>
       </c>
-      <c r="D79" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E79" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F79" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G79" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H79" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I79" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1">
-        <v>38</v>
+      <c r="A80" s="1" t="str">
+        <v>55956</v>
       </c>
       <c r="B80" s="1">
+        <v>38</v>
+      </c>
+      <c r="C80" s="1">
         <v>32</v>
       </c>
-      <c r="C80" s="1">
+      <c r="D80" s="1">
         <v>70</v>
       </c>
-      <c r="D80" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E80" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F80" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G80" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H80" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I80" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1">
+      <c r="A81" s="1" t="str">
+        <v>57933</v>
+      </c>
+      <c r="B81" s="1">
         <v>34</v>
       </c>
-      <c r="B81" s="1">
+      <c r="C81" s="1">
         <v>36</v>
       </c>
-      <c r="C81" s="1">
+      <c r="D81" s="1">
         <v>70</v>
       </c>
-      <c r="D81" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E81" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F81" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G81" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
       </c>
       <c r="H81" s="1" t="str">
-        <v>B-</v>
+        <v>B</v>
+      </c>
+      <c r="I81" s="1" t="str">
+        <v>B</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1">
+      <c r="A82" s="1" t="str">
+        <v>55412</v>
+      </c>
+      <c r="B82" s="1">
         <v>36</v>
       </c>
-      <c r="B82" s="1">
+      <c r="C82" s="1">
         <v>33</v>
       </c>
-      <c r="C82" s="1">
+      <c r="D82" s="1">
         <v>69</v>
       </c>
-      <c r="D82" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E82" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F82" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G82" s="1" t="str">
         <v>B-</v>
@@ -2536,25 +2779,28 @@
       <c r="H82" s="1" t="str">
         <v>B-</v>
       </c>
+      <c r="I82" s="1" t="str">
+        <v>B-</v>
+      </c>
     </row>
     <row r="83">
-      <c r="A83" s="1">
+      <c r="A83" s="1" t="str">
+        <v>57575</v>
+      </c>
+      <c r="B83" s="1">
         <v>28</v>
       </c>
-      <c r="B83" s="1">
+      <c r="C83" s="1">
         <v>41</v>
       </c>
-      <c r="C83" s="1">
+      <c r="D83" s="1">
         <v>69</v>
       </c>
-      <c r="D83" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E83" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F83" s="1" t="str">
-        <v>B-</v>
+        <v>JD</v>
       </c>
       <c r="G83" s="1" t="str">
         <v>B-</v>
@@ -2562,285 +2808,318 @@
       <c r="H83" s="1" t="str">
         <v>B-</v>
       </c>
+      <c r="I83" s="1" t="str">
+        <v>B-</v>
+      </c>
     </row>
     <row r="84">
-      <c r="A84" s="1">
+      <c r="A84" s="1" t="str">
+        <v>58913</v>
+      </c>
+      <c r="B84" s="1">
         <v>32</v>
       </c>
-      <c r="B84" s="1">
+      <c r="C84" s="1">
         <v>36</v>
       </c>
-      <c r="C84" s="1">
+      <c r="D84" s="1">
         <v>68</v>
       </c>
-      <c r="D84" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E84" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F84" s="1" t="str">
-        <v>C+</v>
+        <v>JD</v>
       </c>
       <c r="G84" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
       </c>
       <c r="H84" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
+      </c>
+      <c r="I84" s="1" t="str">
+        <v>B-</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="1">
+      <c r="A85" s="1" t="str">
+        <v>51351</v>
+      </c>
+      <c r="B85" s="1">
         <v>34</v>
       </c>
-      <c r="B85" s="1">
+      <c r="C85" s="1">
         <v>32</v>
       </c>
-      <c r="C85" s="1">
+      <c r="D85" s="1">
         <v>66</v>
       </c>
-      <c r="D85" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E85" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F85" s="1" t="str">
-        <v>C+</v>
+        <v>JD</v>
       </c>
       <c r="G85" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
       </c>
       <c r="H85" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
+      </c>
+      <c r="I85" s="1" t="str">
+        <v>B-</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1">
+      <c r="A86" s="1" t="str">
+        <v>56957</v>
+      </c>
+      <c r="B86" s="1">
         <v>30</v>
       </c>
-      <c r="B86" s="1">
+      <c r="C86" s="1">
         <v>35</v>
       </c>
-      <c r="C86" s="1">
+      <c r="D86" s="1">
         <v>65</v>
       </c>
-      <c r="D86" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E86" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F86" s="1" t="str">
-        <v>C+</v>
+        <v>JD</v>
       </c>
       <c r="G86" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
       </c>
       <c r="H86" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
+      </c>
+      <c r="I86" s="1" t="str">
+        <v>B-</v>
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="1">
+      <c r="A87" s="1" t="str">
+        <v>50204</v>
+      </c>
+      <c r="B87" s="1">
         <v>32</v>
       </c>
-      <c r="B87" s="1">
+      <c r="C87" s="1">
         <v>31</v>
       </c>
-      <c r="C87" s="1">
+      <c r="D87" s="1">
         <v>63</v>
       </c>
-      <c r="D87" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E87" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F87" s="1" t="str">
-        <v>C+</v>
+        <v>JD</v>
       </c>
       <c r="G87" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
       </c>
       <c r="H87" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
+      </c>
+      <c r="I87" s="1" t="str">
+        <v>B-</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="1">
+      <c r="A88" s="1" t="str">
+        <v>53360</v>
+      </c>
+      <c r="B88" s="1">
         <v>34</v>
       </c>
-      <c r="B88" s="1">
+      <c r="C88" s="1">
         <v>29</v>
       </c>
-      <c r="C88" s="1">
+      <c r="D88" s="1">
         <v>63</v>
       </c>
-      <c r="D88" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E88" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F88" s="1" t="str">
-        <v>C+</v>
+        <v>JD</v>
       </c>
       <c r="G88" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
       </c>
       <c r="H88" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
+      </c>
+      <c r="I88" s="1" t="str">
+        <v>B-</v>
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="1">
+      <c r="A89" s="1" t="str">
+        <v>50910</v>
+      </c>
+      <c r="B89" s="1">
         <v>30</v>
       </c>
-      <c r="B89" s="1">
+      <c r="C89" s="1">
         <v>32</v>
       </c>
-      <c r="C89" s="1">
+      <c r="D89" s="1">
         <v>62</v>
       </c>
-      <c r="D89" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E89" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F89" s="1" t="str">
-        <v>C+</v>
+        <v>JD</v>
       </c>
       <c r="G89" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
       </c>
       <c r="H89" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
+      </c>
+      <c r="I89" s="1" t="str">
+        <v>B-</v>
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="1">
+      <c r="A90" s="1" t="str">
+        <v>53483</v>
+      </c>
+      <c r="B90" s="1">
         <v>30</v>
       </c>
-      <c r="B90" s="1">
+      <c r="C90" s="1">
         <v>31</v>
       </c>
-      <c r="C90" s="1">
+      <c r="D90" s="1">
         <v>61</v>
       </c>
-      <c r="D90" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E90" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F90" s="1" t="str">
-        <v>C+</v>
+        <v>JD</v>
       </c>
       <c r="G90" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
       </c>
       <c r="H90" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
+      </c>
+      <c r="I90" s="1" t="str">
+        <v>B-</v>
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="1">
-        <v>30</v>
+      <c r="A91" s="1" t="str">
+        <v>52556</v>
       </c>
       <c r="B91" s="1">
         <v>30</v>
       </c>
       <c r="C91" s="1">
+        <v>30</v>
+      </c>
+      <c r="D91" s="1">
         <v>60</v>
       </c>
-      <c r="D91" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E91" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F91" s="1" t="str">
-        <v>C+</v>
+        <v>JD</v>
       </c>
       <c r="G91" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
       </c>
       <c r="H91" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
+      </c>
+      <c r="I91" s="1" t="str">
+        <v>B-</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1">
+      <c r="A92" s="1" t="str">
+        <v>52944</v>
+      </c>
+      <c r="B92" s="1">
         <v>34</v>
       </c>
-      <c r="B92" s="1">
+      <c r="C92" s="1">
         <v>26</v>
       </c>
-      <c r="C92" s="1">
+      <c r="D92" s="1">
         <v>60</v>
       </c>
-      <c r="D92" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E92" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F92" s="1" t="str">
-        <v>C+</v>
+        <v>JD</v>
       </c>
       <c r="G92" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
       </c>
       <c r="H92" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
+      </c>
+      <c r="I92" s="1" t="str">
+        <v>B-</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="1">
+      <c r="A93" s="1" t="str">
+        <v>52639</v>
+      </c>
+      <c r="B93" s="1">
         <v>30</v>
       </c>
-      <c r="B93" s="1">
+      <c r="C93" s="1">
         <v>29</v>
       </c>
-      <c r="C93" s="1">
+      <c r="D93" s="1">
         <v>59</v>
       </c>
-      <c r="D93" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E93" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F93" s="1" t="str">
-        <v>C+</v>
+        <v>JD</v>
       </c>
       <c r="G93" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
       </c>
       <c r="H93" s="1" t="str">
-        <v>C+</v>
+        <v>B-</v>
+      </c>
+      <c r="I93" s="1" t="str">
+        <v>B-</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="1">
+      <c r="A94" s="1" t="str">
+        <v>55767</v>
+      </c>
+      <c r="B94" s="1">
         <v>34</v>
       </c>
-      <c r="B94" s="1">
+      <c r="C94" s="1">
         <v>21</v>
       </c>
-      <c r="C94" s="1">
+      <c r="D94" s="1">
         <v>55</v>
       </c>
-      <c r="D94" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E94" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F94" s="1" t="str">
-        <v>C+</v>
+        <v>JD</v>
       </c>
       <c r="G94" s="1" t="str">
         <v>C+</v>
@@ -2848,50 +3127,56 @@
       <c r="H94" s="1" t="str">
         <v>C+</v>
       </c>
+      <c r="I94" s="1" t="str">
+        <v>C+</v>
+      </c>
     </row>
     <row r="95">
-      <c r="A95" s="1">
+      <c r="A95" s="1" t="str">
+        <v>55124</v>
+      </c>
+      <c r="B95" s="1">
         <v>34</v>
       </c>
-      <c r="B95" s="1">
+      <c r="C95" s="1">
         <v>17</v>
       </c>
-      <c r="C95" s="1">
+      <c r="D95" s="1">
         <v>51</v>
       </c>
-      <c r="D95" s="1" t="str">
-        <v>GRD</v>
-      </c>
       <c r="E95" s="1" t="str">
-        <v>JD</v>
+        <v>GRD</v>
       </c>
       <c r="F95" s="1" t="str">
+        <v>JD</v>
+      </c>
+      <c r="G95" s="1" t="str">
         <v>C</v>
       </c>
-      <c r="G95" s="1" t="str">
-        <v>F</v>
-      </c>
       <c r="H95" s="1" t="str">
+        <v>C+</v>
+      </c>
+      <c r="I95" s="1" t="str">
         <v>C</v>
       </c>
     </row>
     <row r="96">
-      <c r="C96" s="1">
+      <c r="D96" s="1">
         <v>77.8723404255319</v>
       </c>
-      <c r="F96" s="1" t="str">
-        <v>B</v>
-      </c>
       <c r="G96" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
       </c>
       <c r="H96" s="1" t="str">
-        <v>B</v>
+        <v>B+</v>
+      </c>
+      <c r="I96" s="1" t="str">
+        <v>B+</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H96"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I96"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>